<commit_message>
Added code to store test reports to shared path
</commit_message>
<xml_diff>
--- a/bin/testdata/furnitureData.xlsx
+++ b/bin/testdata/furnitureData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>MenuFromHome</t>
   </si>
@@ -168,6 +168,21 @@
   </si>
   <si>
     <t>70982197</t>
+  </si>
+  <si>
+    <t>48338495</t>
+  </si>
+  <si>
+    <t>97689688</t>
+  </si>
+  <si>
+    <t>40670685</t>
+  </si>
+  <si>
+    <t>80834542</t>
+  </si>
+  <si>
+    <t>41655678</t>
   </si>
 </sst>
 </file>
@@ -548,7 +563,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated shared folder path
</commit_message>
<xml_diff>
--- a/bin/testdata/furnitureData.xlsx
+++ b/bin/testdata/furnitureData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>MenuFromHome</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>41655678</t>
+  </si>
+  <si>
+    <t>4191853</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated code to add screenshots to th report
</commit_message>
<xml_diff>
--- a/bin/testdata/furnitureData.xlsx
+++ b/bin/testdata/furnitureData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>MenuFromHome</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>41655678</t>
+  </si>
+  <si>
+    <t>73343227</t>
+  </si>
+  <si>
+    <t>30677524</t>
   </si>
 </sst>
 </file>
@@ -563,7 +569,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>